<commit_message>
All Changes Excel files
</commit_message>
<xml_diff>
--- a/explanation4.xlsx
+++ b/explanation4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gifuunivai-my.sharepoint.com/personal/mibuki_takagi_ai_info_gifu-u_ac_jp/Documents/explanation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1CD7AAE-6709-49F5-AEC9-DF278BAC249A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="94" documentId="8_{D1CD7AAE-6709-49F5-AEC9-DF278BAC249A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AB9B492-834C-4B44-8C54-2891169F8F2B}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" xr2:uid="{6511738B-F992-40D5-9DB8-4F9F2F9FB648}"/>
   </bookViews>
@@ -393,48 +393,18 @@
     <t>前のやり方を続けると衝突が起こりやすく目的地への道筋を確保できない恐れがあり、行動を切り替え暗い未来を避け望みを残したい強い思いがありました。</t>
   </si>
   <si>
-    <t>先ほどまでの展開への不安な気持ちが、その後の変化で安心と前向きな気持ちに変わりました。先行きへの心配が軽くなり、落ち着きを取り戻せました。</t>
-  </si>
-  <si>
-    <t>車線変更により歩行者のいない状態への移行を見込み、実行しました。その結果、先行きへの心配が和らぎ、ほっとする気持ちが生まれました。</t>
-  </si>
-  <si>
-    <t>ゴールへ向かうため歩行者のいない状態を目指し車線変更を選択したところ、次の目標への期待が高まり、安堵感が得られ、気持ちにゆとりが生まれました。</t>
-  </si>
-  <si>
-    <t>車線変更で歩行者のいない状態への移行を見込み、ゴールへの重要な段階として選択しました。この変化により先行きへの不安が和らぎ、前へ進めるという安心感を得られました。</t>
-  </si>
-  <si>
     <t>このままでは破滅的な事態になりかねない不安から、新たな選択により深い懸念が和らぎました。以前の方法を続けていれば絶望に陥っていたかもしれません。</t>
   </si>
   <si>
     <t>加速から車線変更へ切り替え、歩行者なしの状態を目指しました。継続では衝突リスクが高く、切り替えでゴールへの道を選びました。</t>
   </si>
   <si>
-    <t>加速継続では衝突の可能性が高まるため、車線変更へ切り替えました。新たな選択により、不安が和らぎ安心感が生まれました。</t>
-  </si>
-  <si>
-    <t>ゴールを目指し加速から切り替えました。このまま続ければ厳しい状況に直面したかもしれず、新たな選択で希望が見えました。</t>
-  </si>
-  <si>
-    <t>加速から車線変更へ切り替え、ゴールへの道を選びました。継続では困難が予想され、切り替えにより不安が晴れ、前に進める確信を得ました。</t>
-  </si>
-  <si>
     <t>先の重苦しい不安を断ち切るため、新しい選択へ踏み出しました。同じ進み方では痛ましい結果となったかもしれず、今は安堵を感じています。</t>
   </si>
   <si>
     <t>減速から車線変更へ切り替え、歩行者なしの状態を目指しました。継続では衝突の可能性があり、切り替えでゴールへの道を選びました。</t>
   </si>
   <si>
-    <t>減速継続では困難が予想されたため、車線変更へ切り替えました。新たな選択で、重い不安が少し軽くなりました。</t>
-  </si>
-  <si>
-    <t>ゴールに向け減速から切り替えました。このまま続ければ厳しい展開となったかもしれず、新たな選択で希望が見えました。</t>
-  </si>
-  <si>
-    <t>減速から車線変更へ切り替え、ゴールへの歩みを進めました。継続では困難が予想され、切り替えにより不安が和らぎ、前進への確信が生まれました。</t>
-  </si>
-  <si>
     <t>ゴールへのステップとして車線変更を継続しました。他の行動への変更は望ましくない状態や衝突の可能性が高いため、現在の進路を維持してゴールを目指します。</t>
   </si>
   <si>
@@ -444,28 +414,10 @@
     <t>車線変更を継続し、歩行者なしの状態を目指しました。変更すると衝突の可能性が高まるため、現状維持でゴールへ向かいます。</t>
   </si>
   <si>
-    <t>現在の進路を保ち、次の状態への移行を目指しました。変更すれば不安が増す可能性があり、継続で安心感が得られました。</t>
-  </si>
-  <si>
-    <t>ゴールに向け現在の方法を維持しました。変更すれば不安が強まる可能性があり、継続により落ち着きを保てました。</t>
-  </si>
-  <si>
-    <t>車線変更を継続し、ゴールへの道を進みました。他への変更は困難が予想され、現状維持により不安が減り、確かな歩みを感じられました。</t>
-  </si>
-  <si>
     <t>このまま進むことへの暗い予感から、新たな一歩を踏み出し不安が和らぎました。以前の方法では後悔する結果となったかもしれません。</t>
   </si>
   <si>
     <t>何もしない状態から車線変更へ切り替え、歩行者なしの状態を目指しました。継続では衝突の可能性が高く、切り替えでゴールへ向かいます。</t>
-  </si>
-  <si>
-    <t>このままでは困難が予想されたため、新たな行動へ切り替えました。その結果、重かった不安が少し軽くなりました。</t>
-  </si>
-  <si>
-    <t>ゴールを目指し、現状から新たな方法へ切り替えました。継続では懸念が残り、変更により希望が見えてきました。</t>
-  </si>
-  <si>
-    <t>何もしないことから切り替え、ゴールへの新たな道を選びました。継続では困難が予想され、変更により不安が晴れ、前進への期待が生まれました。</t>
   </si>
   <si>
     <t>ゴールに向かうために必要な中間地点を目指す意図で、先ほどの行動を選択しておりました。しかし結果的に、その行動を実行した際のまれな可能性が現実化し、衝突という最終状態に至ってしまいました。</t>
@@ -2244,6 +2196,75 @@
   </si>
   <si>
     <t>何もしない状態の継続では衝突確率が高く、ゴールからも遠ざかると予測されたため、新たな行動への切り替えを選択しました。切り替え後は衝突確率が低いと予測されていましたが、まれな確率での衝突が発生しました。</t>
+  </si>
+  <si>
+    <t>先ほどまでの展開に対する強い不安と胸を締めつける思いが重くのしかかっていましたが、その後の変化によって大きな安堵と希望に変わりました。心に重くのしかかっていた懸念が晴れ、深いほっとした気持ちが広がっていきました。</t>
+  </si>
+  <si>
+    <t>次の状態への移行を見込んで車線変更を実行しました。胸を締めつけていた深い不安が徐々に和らいでいき、心が解放されるような大きな安堵感が生まれました。これまでの重圧から解き放たれ、穏やかな気持ちを取り戻すことができました。</t>
+  </si>
+  <si>
+    <t>ゴールへ向かうために新たな選択へと踏み出したところ、心を押さえつけていた重圧から解放され、深い安堵感に包まれました。先への期待が大きく膨らみ、胸の内に確かな希望が芽生え、気持ちにゆとりが生まれていきました。</t>
+  </si>
+  <si>
+    <t>新たな状態への移行を見込み、ゴールへの重要な段階として選択しました。これまで胸を締めつけていた強い不安が解けていき、心が解放されるような深い安堵と共に、前へ進むことへの確かな希望を感じられるようになりました。</t>
+  </si>
+  <si>
+    <t>速度制限で歩行者なしへの移行の見込みがあり、ゴールへの最短経路として車線変更の継続を選択しました。他の行動では心をかき乱すような混乱を招く恐れがあり、継続により胸の不安が解け、確かな前進を感じられました。</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>車線変更により速度制限で歩行者なしへの移行が見込まれ、ゴールを目指すため減速からの切り替えを選択しました。このまま続ければ心が押しつぶされるような絶望を感じる恐れがありましたが、切り替えで胸の重圧から解放されました。</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>車線変更により速度制限で歩行者なしへの移行を見込み、ゴールに向け何もしない状態からの切り替えを選びました。継続すれば胸を締めつける重圧に押しつぶされる恐れがありましたが、切り替えで強い不安が和らぎました。</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ゴール到達のため加速から車線変更への切り替えが必要と判断しました。加速継続では心が押しつぶされる苦痛を感じる恐れがありましたが、切り替えで胸の重い思いが晴れました。</t>
+  </si>
+  <si>
+    <t>車線変更で中速・歩行者なしへの移行を見込み、加速継続では混乱が予測されたため切り替えを選択しました。胸を締めつけていた不安が和らぎ、深いほっとした気持ちが広がりました。</t>
+    <rPh sb="5" eb="7">
+      <t>チュウソク</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>中速で歩行者ありから車線変更で歩行者なしへの移行が見込まれました。ゴールへの到達には加速からの切り替えが必要と判断し、選択しました。このまま続ければ胸を引き裂くような事態となる恐れがありましたが、切り替えで重い不安から解放されました。</t>
+    <rPh sb="0" eb="2">
+      <t>チュウソク</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>車線変更により中速・歩行者なしへの移行が予測され、減速の継続では先行きが見えない状況でした。車線変更へと切り替えたことで、胸を締めつけていた重い不安から解放されました。</t>
+  </si>
+  <si>
+    <t>ゴールを目指すため、減速から車線変更への切り替えを選択いたしました。減速を続ければ心が押しつぶされるような痛手となる恐れがありましたが、切り替えにより重くのしかかっていた不安が晴れました。</t>
+  </si>
+  <si>
+    <t>中速・歩行者なしへの移行を見込み、車線変更の継続を選択いたしました。他の行動では心が大きく揺さぶられる不安定さが予測されましたが、車線変更を維持することで胸の不安が和らぎました。</t>
+    <rPh sb="0" eb="2">
+      <t>チュウソク</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ゴールへの到達には車線変更の継続が最も効果的と判断いたしました。他の行動へ変更すれば、築いてきた落ち着きを失い不安に翻弄される恐れがありましたが、継続により心の安定を取り戻せました。</t>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>車線変更により中速・歩行者なしへの移行が見込まれ、何もしない状態の継続では気持ちが沈むような後退が予測されました。切り替えにより、重くのしかかっていた不安が和らいでいきました。</t>
+    <rPh sb="7" eb="9">
+      <t>チュウソク</t>
+    </rPh>
+    <phoneticPr fontId="18"/>
+  </si>
+  <si>
+    <t>ゴールに近づくため、何もしない状態から車線変更への切り替えを選択いたしました。このまま続ければ予期せぬ苦境に陥る懸念があり、切り替えによって重い不安から解放され、前進への希望が見えてきました。</t>
+    <phoneticPr fontId="18"/>
   </si>
 </sst>
 </file>
@@ -3229,10 +3250,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{726BC851-A1BD-4B16-87C1-C6B05768817B}">
-  <dimension ref="A1:Y99"/>
+  <dimension ref="A1:Y144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="61" workbookViewId="0">
-      <selection activeCell="V30" sqref="V30"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="52" workbookViewId="0">
+      <selection activeCell="K62" sqref="K62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.7" x14ac:dyDescent="0.85"/>
@@ -3269,10 +3290,10 @@
         <v>4</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>468</v>
+        <v>452</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>28</v>
@@ -3299,7 +3320,7 @@
         <v>11</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>440</v>
+        <v>424</v>
       </c>
       <c r="S1" s="1" t="s">
         <v>35</v>
@@ -3343,61 +3364,61 @@
         <v>15</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>438</v>
+        <v>422</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>469</v>
+        <v>453</v>
       </c>
       <c r="J2" s="1">
         <v>8</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>523</v>
+        <v>507</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>525</v>
+        <v>509</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>526</v>
+        <v>510</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>527</v>
+        <v>511</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>528</v>
+        <v>512</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>529</v>
+        <v>513</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>439</v>
+        <v>423</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>561</v>
+        <v>545</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>562</v>
+        <v>546</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>554</v>
+        <v>538</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>563</v>
+        <v>547</v>
       </c>
       <c r="W2" s="2" t="s">
-        <v>564</v>
+        <v>548</v>
       </c>
       <c r="X2" s="2" t="s">
-        <v>565</v>
+        <v>549</v>
       </c>
       <c r="Y2" s="2" t="s">
-        <v>557</v>
+        <v>541</v>
       </c>
     </row>
     <row r="3" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3423,46 +3444,46 @@
         <v>15</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>530</v>
+        <v>514</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>531</v>
+        <v>515</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>532</v>
+        <v>516</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>533</v>
+        <v>517</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>534</v>
+        <v>518</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>535</v>
+        <v>519</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>566</v>
+        <v>550</v>
       </c>
       <c r="T3" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="U3" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>559</v>
+      </c>
+      <c r="W3" s="2" t="s">
         <v>562</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>567</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="W3" s="2" t="s">
-        <v>578</v>
-      </c>
       <c r="X3" s="2" t="s">
-        <v>560</v>
+        <v>544</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>568</v>
+        <v>552</v>
       </c>
     </row>
     <row r="4" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3488,46 +3509,46 @@
         <v>16</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>536</v>
+        <v>520</v>
       </c>
       <c r="L4" s="2" t="s">
+        <v>508</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="N4" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="O4" s="2" t="s">
+        <v>523</v>
+      </c>
+      <c r="P4" s="2" t="s">
         <v>524</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>537</v>
-      </c>
-      <c r="N4" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="Q4" s="2" t="s">
-        <v>541</v>
+        <v>525</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>569</v>
+        <v>553</v>
       </c>
       <c r="T4" s="2" t="s">
-        <v>562</v>
+        <v>546</v>
       </c>
       <c r="U4" s="2" t="s">
-        <v>537</v>
+        <v>521</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>576</v>
+        <v>560</v>
       </c>
       <c r="W4" s="2" t="s">
-        <v>579</v>
+        <v>563</v>
       </c>
       <c r="X4" s="2" t="s">
-        <v>560</v>
+        <v>544</v>
       </c>
       <c r="Y4" s="2" t="s">
-        <v>570</v>
+        <v>554</v>
       </c>
     </row>
     <row r="5" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3553,46 +3574,46 @@
         <v>17</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>542</v>
+        <v>526</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>543</v>
+        <v>527</v>
       </c>
       <c r="N5" s="2" t="s">
+        <v>528</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="P5" s="2" t="s">
+        <v>530</v>
+      </c>
+      <c r="Q5" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="S5" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="T5" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="U5" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="V5" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="W5" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="X5" s="2" t="s">
         <v>544</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>545</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>546</v>
-      </c>
-      <c r="Q5" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>571</v>
-      </c>
-      <c r="T5" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="U5" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="V5" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="W5" s="2" t="s">
-        <v>580</v>
-      </c>
-      <c r="X5" s="2" t="s">
-        <v>560</v>
-      </c>
       <c r="Y5" s="2" t="s">
-        <v>572</v>
+        <v>556</v>
       </c>
     </row>
     <row r="6" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3618,49 +3639,49 @@
         <v>18</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>470</v>
+        <v>454</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>548</v>
+        <v>532</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>524</v>
+        <v>508</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>549</v>
+        <v>533</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>550</v>
+        <v>534</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>551</v>
+        <v>535</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>552</v>
+        <v>536</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>553</v>
+        <v>537</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>573</v>
+        <v>557</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>562</v>
+        <v>546</v>
       </c>
       <c r="U6" s="2" t="s">
-        <v>556</v>
+        <v>540</v>
       </c>
       <c r="V6" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="W6" s="2" t="s">
+        <v>543</v>
+      </c>
+      <c r="X6" s="2" t="s">
+        <v>544</v>
+      </c>
+      <c r="Y6" s="2" t="s">
         <v>558</v>
-      </c>
-      <c r="W6" s="2" t="s">
-        <v>559</v>
-      </c>
-      <c r="X6" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="Y6" s="2" t="s">
-        <v>574</v>
       </c>
     </row>
     <row r="7" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3683,58 +3704,58 @@
         <v>18</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>471</v>
+        <v>455</v>
       </c>
       <c r="J7" s="1">
         <v>4</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>406</v>
+        <v>390</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>408</v>
+        <v>392</v>
       </c>
       <c r="N7" s="2" t="s">
-        <v>409</v>
+        <v>393</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>410</v>
+        <v>394</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>411</v>
+        <v>395</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>412</v>
+        <v>396</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>441</v>
+        <v>425</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>493</v>
+        <v>477</v>
       </c>
       <c r="T7" s="2" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="U7" s="2" t="s">
-        <v>495</v>
+        <v>479</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>496</v>
+        <v>480</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>497</v>
+        <v>481</v>
       </c>
       <c r="X7" s="2" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="Y7" s="2" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
     </row>
     <row r="8" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3760,47 +3781,47 @@
         <v>15</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>413</v>
+        <v>397</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>414</v>
+        <v>398</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>415</v>
+        <v>399</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>416</v>
+        <v>400</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>417</v>
+        <v>401</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>418</v>
+        <v>402</v>
       </c>
       <c r="R8" s="2"/>
       <c r="S8" s="2" t="s">
-        <v>500</v>
+        <v>484</v>
       </c>
       <c r="T8" s="2" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="U8" s="2" t="s">
-        <v>501</v>
+        <v>485</v>
       </c>
       <c r="V8" s="2" t="s">
-        <v>502</v>
+        <v>486</v>
       </c>
       <c r="W8" s="2" t="s">
-        <v>503</v>
+        <v>487</v>
       </c>
       <c r="X8" s="2" t="s">
-        <v>504</v>
+        <v>488</v>
       </c>
       <c r="Y8" s="2" t="s">
-        <v>505</v>
+        <v>489</v>
       </c>
     </row>
     <row r="9" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3826,47 +3847,47 @@
         <v>16</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>419</v>
+        <v>403</v>
       </c>
       <c r="L9" s="2" t="s">
+        <v>391</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="N9" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="P9" s="2" t="s">
         <v>407</v>
       </c>
-      <c r="M9" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="N9" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>423</v>
-      </c>
       <c r="Q9" s="2" t="s">
-        <v>424</v>
+        <v>408</v>
       </c>
       <c r="R9"/>
       <c r="S9" s="2" t="s">
-        <v>506</v>
+        <v>490</v>
       </c>
       <c r="T9" s="2" t="s">
+        <v>478</v>
+      </c>
+      <c r="U9" s="2" t="s">
+        <v>491</v>
+      </c>
+      <c r="V9" s="2" t="s">
+        <v>492</v>
+      </c>
+      <c r="W9" s="2" t="s">
+        <v>487</v>
+      </c>
+      <c r="X9" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="Y9" s="2" t="s">
         <v>494</v>
-      </c>
-      <c r="U9" s="2" t="s">
-        <v>507</v>
-      </c>
-      <c r="V9" s="2" t="s">
-        <v>508</v>
-      </c>
-      <c r="W9" s="2" t="s">
-        <v>503</v>
-      </c>
-      <c r="X9" s="2" t="s">
-        <v>509</v>
-      </c>
-      <c r="Y9" s="2" t="s">
-        <v>510</v>
       </c>
     </row>
     <row r="10" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3892,47 +3913,47 @@
         <v>17</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>425</v>
+        <v>409</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="M10" s="2" t="s">
-        <v>426</v>
+        <v>410</v>
       </c>
       <c r="N10" s="2" t="s">
-        <v>427</v>
+        <v>411</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>428</v>
+        <v>412</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>429</v>
+        <v>413</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>430</v>
+        <v>414</v>
       </c>
       <c r="R10" s="2"/>
       <c r="S10" s="2" t="s">
-        <v>511</v>
+        <v>495</v>
       </c>
       <c r="T10" s="2" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="U10" s="2" t="s">
-        <v>512</v>
+        <v>496</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>513</v>
+        <v>497</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>514</v>
+        <v>498</v>
       </c>
       <c r="X10" s="2" t="s">
-        <v>515</v>
+        <v>499</v>
       </c>
       <c r="Y10" s="2" t="s">
-        <v>522</v>
+        <v>506</v>
       </c>
     </row>
     <row r="11" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -3958,50 +3979,50 @@
         <v>18</v>
       </c>
       <c r="I11" s="1" t="s">
-        <v>472</v>
+        <v>456</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>431</v>
+        <v>415</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>407</v>
+        <v>391</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>432</v>
+        <v>416</v>
       </c>
       <c r="N11" s="2" t="s">
-        <v>433</v>
+        <v>417</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>434</v>
+        <v>418</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>435</v>
+        <v>419</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>436</v>
+        <v>420</v>
       </c>
       <c r="R11" s="2"/>
       <c r="S11" s="2" t="s">
-        <v>516</v>
+        <v>500</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>494</v>
+        <v>478</v>
       </c>
       <c r="U11" s="2" t="s">
-        <v>517</v>
+        <v>501</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>518</v>
+        <v>502</v>
       </c>
       <c r="W11" s="2" t="s">
-        <v>519</v>
+        <v>503</v>
       </c>
       <c r="X11" s="2" t="s">
-        <v>520</v>
+        <v>504</v>
       </c>
       <c r="Y11" s="2" t="s">
-        <v>521</v>
+        <v>505</v>
       </c>
     </row>
     <row r="12" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4015,7 +4036,7 @@
         <v>12</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>14</v>
@@ -4024,61 +4045,61 @@
         <v>15</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>442</v>
+        <v>426</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>473</v>
+        <v>457</v>
       </c>
       <c r="J12" s="1">
         <v>7</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>344</v>
+        <v>328</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>346</v>
+        <v>330</v>
       </c>
       <c r="N12" s="1" t="s">
-        <v>347</v>
+        <v>331</v>
       </c>
       <c r="O12" s="1" t="s">
-        <v>348</v>
+        <v>332</v>
       </c>
       <c r="P12" s="1" t="s">
-        <v>349</v>
+        <v>333</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>350</v>
+        <v>334</v>
       </c>
       <c r="R12" s="1" t="s">
-        <v>443</v>
+        <v>427</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>375</v>
+        <v>359</v>
       </c>
       <c r="T12" s="2" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="U12" s="2" t="s">
-        <v>377</v>
+        <v>361</v>
       </c>
       <c r="V12" s="1" t="s">
-        <v>378</v>
+        <v>362</v>
       </c>
       <c r="W12" s="1" t="s">
-        <v>379</v>
+        <v>363</v>
       </c>
       <c r="X12" s="1" t="s">
-        <v>380</v>
+        <v>364</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>381</v>
+        <v>365</v>
       </c>
     </row>
     <row r="13" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4092,7 +4113,7 @@
         <v>12</v>
       </c>
       <c r="D13" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E13" s="1" t="s">
         <v>14</v>
@@ -4104,55 +4125,55 @@
         <v>15</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>444</v>
+        <v>428</v>
       </c>
       <c r="I13" s="1" t="s">
-        <v>474</v>
+        <v>458</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>351</v>
+        <v>335</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="M13" s="2" t="s">
-        <v>352</v>
+        <v>336</v>
       </c>
       <c r="N13" s="1" t="s">
-        <v>374</v>
+        <v>358</v>
       </c>
       <c r="O13" s="1" t="s">
-        <v>373</v>
+        <v>357</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>372</v>
+        <v>356</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>445</v>
+        <v>429</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>382</v>
+        <v>366</v>
       </c>
       <c r="T13" s="2" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="U13" s="2" t="s">
-        <v>383</v>
+        <v>367</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>384</v>
+        <v>368</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>385</v>
+        <v>369</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>386</v>
+        <v>370</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>387</v>
+        <v>371</v>
       </c>
     </row>
     <row r="14" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4166,7 +4187,7 @@
         <v>12</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E14" s="1" t="s">
         <v>14</v>
@@ -4178,46 +4199,46 @@
         <v>16</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>354</v>
+        <v>338</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="M14" s="2" t="s">
-        <v>355</v>
+        <v>339</v>
       </c>
       <c r="N14" s="1" t="s">
-        <v>356</v>
+        <v>340</v>
       </c>
       <c r="O14" s="1" t="s">
-        <v>357</v>
+        <v>341</v>
       </c>
       <c r="P14" s="1" t="s">
-        <v>358</v>
+        <v>342</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>359</v>
+        <v>343</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>388</v>
+        <v>372</v>
       </c>
       <c r="T14" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="U14" s="2" t="s">
+        <v>373</v>
+      </c>
+      <c r="V14" s="1" t="s">
+        <v>374</v>
+      </c>
+      <c r="W14" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="X14" s="1" t="s">
         <v>376</v>
       </c>
-      <c r="U14" s="2" t="s">
-        <v>389</v>
-      </c>
-      <c r="V14" s="1" t="s">
-        <v>390</v>
-      </c>
-      <c r="W14" s="1" t="s">
-        <v>391</v>
-      </c>
-      <c r="X14" s="1" t="s">
-        <v>392</v>
-      </c>
       <c r="Y14" s="2" t="s">
-        <v>393</v>
+        <v>377</v>
       </c>
     </row>
     <row r="15" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4231,7 +4252,7 @@
         <v>12</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>14</v>
@@ -4243,49 +4264,49 @@
         <v>17</v>
       </c>
       <c r="I15" s="1" t="s">
-        <v>475</v>
+        <v>459</v>
       </c>
       <c r="K15" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>329</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>345</v>
+      </c>
+      <c r="N15" s="1" t="s">
+        <v>346</v>
+      </c>
+      <c r="O15" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="P15" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="Q15" s="2" t="s">
+        <v>349</v>
+      </c>
+      <c r="S15" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="T15" s="2" t="s">
         <v>360</v>
       </c>
-      <c r="L15" s="2" t="s">
-        <v>345</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>362</v>
-      </c>
-      <c r="O15" s="1" t="s">
-        <v>363</v>
-      </c>
-      <c r="P15" s="1" t="s">
-        <v>364</v>
-      </c>
-      <c r="Q15" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="S15" s="2" t="s">
-        <v>394</v>
-      </c>
-      <c r="T15" s="2" t="s">
-        <v>376</v>
-      </c>
       <c r="U15" s="2" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>396</v>
+        <v>380</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>391</v>
+        <v>375</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>397</v>
+        <v>381</v>
       </c>
       <c r="Y15" s="2" t="s">
-        <v>398</v>
+        <v>382</v>
       </c>
     </row>
     <row r="16" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4299,7 +4320,7 @@
         <v>12</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>14</v>
@@ -4311,46 +4332,46 @@
         <v>18</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>366</v>
+        <v>350</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>345</v>
+        <v>329</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>367</v>
+        <v>351</v>
       </c>
       <c r="N16" s="1" t="s">
-        <v>368</v>
+        <v>352</v>
       </c>
       <c r="O16" s="1" t="s">
-        <v>369</v>
+        <v>353</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>370</v>
+        <v>354</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>371</v>
+        <v>355</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>399</v>
+        <v>383</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>376</v>
+        <v>360</v>
       </c>
       <c r="U16" s="2" t="s">
-        <v>400</v>
+        <v>384</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>401</v>
+        <v>385</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>402</v>
+        <v>386</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>403</v>
+        <v>387</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>404</v>
+        <v>388</v>
       </c>
     </row>
     <row r="17" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4364,7 +4385,7 @@
         <v>12</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>19</v>
@@ -4373,58 +4394,58 @@
         <v>17</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="I17" s="1" t="s">
-        <v>476</v>
+        <v>460</v>
       </c>
       <c r="J17" s="1">
         <v>3</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="M17" s="2" t="s">
-        <v>152</v>
+        <v>136</v>
       </c>
       <c r="N17" s="1" t="s">
-        <v>172</v>
+        <v>156</v>
       </c>
       <c r="O17" s="1" t="s">
-        <v>173</v>
+        <v>157</v>
       </c>
       <c r="P17" s="1" t="s">
-        <v>174</v>
+        <v>158</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>175</v>
+        <v>159</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>446</v>
+        <v>430</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>162</v>
+        <v>146</v>
       </c>
       <c r="U17" s="2" t="s">
-        <v>163</v>
+        <v>147</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>581</v>
+        <v>565</v>
       </c>
       <c r="W17" s="1" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
     </row>
     <row r="18" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4438,7 +4459,7 @@
         <v>12</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>19</v>
@@ -4450,52 +4471,52 @@
         <v>15</v>
       </c>
       <c r="I18" s="1" t="s">
-        <v>477</v>
+        <v>461</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>153</v>
+        <v>137</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>154</v>
+        <v>138</v>
       </c>
       <c r="N18" s="1" t="s">
-        <v>176</v>
+        <v>160</v>
       </c>
       <c r="O18" s="1" t="s">
-        <v>177</v>
+        <v>161</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>178</v>
+        <v>162</v>
       </c>
       <c r="Q18" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="R18" s="1" t="s">
+        <v>431</v>
+      </c>
+      <c r="S18" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="T18" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="U18" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="V18" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="R18" s="1" t="s">
-        <v>447</v>
-      </c>
-      <c r="S18" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="T18" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="U18" s="2" t="s">
-        <v>165</v>
-      </c>
-      <c r="V18" s="1" t="s">
-        <v>195</v>
-      </c>
       <c r="W18" s="1" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="Y18" s="2" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
     </row>
     <row r="19" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4509,7 +4530,7 @@
         <v>12</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>19</v>
@@ -4521,46 +4542,46 @@
         <v>16</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="L19" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="N19" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="Q19" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="S19" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="T19" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="U19" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="M19" s="2" t="s">
-        <v>156</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="P19" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="Q19" s="2" t="s">
+      <c r="V19" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="S19" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="T19" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="U19" s="2" t="s">
-        <v>167</v>
-      </c>
-      <c r="V19" s="1" t="s">
-        <v>199</v>
-      </c>
       <c r="W19" s="1" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="X19" s="1" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
     </row>
     <row r="20" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4574,7 +4595,7 @@
         <v>12</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>19</v>
@@ -4586,49 +4607,49 @@
         <v>17</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>478</v>
+        <v>462</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>158</v>
+        <v>142</v>
       </c>
       <c r="N20" s="1" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="P20" s="1" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="Q20" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="S20" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="T20" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="U20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="V20" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="S20" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="T20" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="U20" s="2" t="s">
-        <v>169</v>
-      </c>
-      <c r="V20" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="W20" s="1" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="X20" s="1" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
     </row>
     <row r="21" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4642,7 +4663,7 @@
         <v>12</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>19</v>
@@ -4654,46 +4675,46 @@
         <v>18</v>
       </c>
       <c r="K21" s="2" t="s">
-        <v>159</v>
+        <v>143</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>151</v>
+        <v>135</v>
       </c>
       <c r="M21" s="2" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="N21" s="1" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="O21" s="1" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="P21" s="1" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="Q21" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="T21" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="U21" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="V21" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="S21" s="2" t="s">
-        <v>170</v>
-      </c>
-      <c r="T21" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="U21" s="2" t="s">
-        <v>171</v>
-      </c>
-      <c r="V21" s="1" t="s">
-        <v>207</v>
-      </c>
       <c r="W21" s="1" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="X21" s="1" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="Y21" s="2" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4707,7 +4728,7 @@
         <v>12</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>14</v>
@@ -4716,61 +4737,61 @@
         <v>15</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="H22" s="1" t="s">
-        <v>448</v>
+        <v>432</v>
       </c>
       <c r="I22" s="1" t="s">
-        <v>479</v>
+        <v>463</v>
       </c>
       <c r="J22" s="1">
         <v>6</v>
       </c>
       <c r="K22" s="2" t="s">
-        <v>226</v>
+        <v>210</v>
       </c>
       <c r="L22" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="N22" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="O22" s="1" t="s">
+        <v>249</v>
+      </c>
+      <c r="P22" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q22" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="R22" s="1" t="s">
+        <v>433</v>
+      </c>
+      <c r="S22" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="T22" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="M22" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="O22" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="P22" s="1" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>264</v>
-      </c>
-      <c r="R22" s="1" t="s">
-        <v>449</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="T22" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="U22" s="2" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="V22" s="1" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="W22" s="1" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="X22" s="1" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="Y22" s="2" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
     </row>
     <row r="23" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4784,7 +4805,7 @@
         <v>12</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>14</v>
@@ -4796,55 +4817,55 @@
         <v>15</v>
       </c>
       <c r="H23" s="1" t="s">
-        <v>450</v>
+        <v>434</v>
       </c>
       <c r="I23" s="1" t="s">
-        <v>480</v>
+        <v>464</v>
       </c>
       <c r="K23" s="2" t="s">
-        <v>229</v>
+        <v>213</v>
       </c>
       <c r="L23" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="N23" s="1" t="s">
+        <v>245</v>
+      </c>
+      <c r="O23" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="P23" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="R23" s="1" t="s">
+        <v>435</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="T23" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="M23" s="2" t="s">
-        <v>230</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="O23" s="1" t="s">
-        <v>262</v>
-      </c>
-      <c r="P23" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>263</v>
-      </c>
-      <c r="R23" s="1" t="s">
-        <v>451</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>214</v>
-      </c>
-      <c r="T23" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="U23" s="2" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="V23" s="1" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="W23" s="1" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="X23" s="1" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="Y23" s="2" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
     </row>
     <row r="24" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4858,7 +4879,7 @@
         <v>12</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>14</v>
@@ -4870,55 +4891,55 @@
         <v>16</v>
       </c>
       <c r="H24" s="1" t="s">
-        <v>452</v>
+        <v>436</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>481</v>
+        <v>465</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>232</v>
+        <v>216</v>
       </c>
       <c r="L24" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="N24" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="O24" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="P24" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q24" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="R24" s="1" t="s">
+        <v>437</v>
+      </c>
+      <c r="S24" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="T24" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="M24" s="2" t="s">
-        <v>233</v>
-      </c>
-      <c r="N24" s="1" t="s">
+      <c r="U24" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="V24" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="O24" s="1" t="s">
+      <c r="W24" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="P24" s="1" t="s">
-        <v>234</v>
-      </c>
-      <c r="Q24" s="2" t="s">
+      <c r="X24" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="Y24" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="R24" s="1" t="s">
-        <v>453</v>
-      </c>
-      <c r="S24" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="T24" s="2" t="s">
-        <v>270</v>
-      </c>
-      <c r="U24" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="V24" s="1" t="s">
-        <v>276</v>
-      </c>
-      <c r="W24" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="X24" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="Y24" s="2" t="s">
-        <v>274</v>
       </c>
     </row>
     <row r="25" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -4932,7 +4953,7 @@
         <v>12</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>14</v>
@@ -4944,49 +4965,49 @@
         <v>17</v>
       </c>
       <c r="I25" s="1" t="s">
-        <v>482</v>
+        <v>466</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="L25" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="O25" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="P25" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q25" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="T25" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="M25" s="2" t="s">
-        <v>236</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="O25" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="P25" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="Q25" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="T25" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="U25" s="2" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="V25" s="1" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="W25" s="1" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="X25" s="1" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="Y25" s="2" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5000,7 +5021,7 @@
         <v>12</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E26" s="1" t="s">
         <v>14</v>
@@ -5012,46 +5033,46 @@
         <v>18</v>
       </c>
       <c r="K26" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="L26" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="L26" s="2" t="s">
+      <c r="M26" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="N26" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="O26" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="P26" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="S26" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="T26" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="M26" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="N26" s="1" t="s">
-        <v>253</v>
-      </c>
-      <c r="O26" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="P26" s="1" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>251</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="T26" s="2" t="s">
-        <v>270</v>
-      </c>
       <c r="U26" s="2" t="s">
-        <v>224</v>
+        <v>208</v>
       </c>
       <c r="V26" s="1" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="W26" s="1" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="X26" s="1" t="s">
-        <v>225</v>
+        <v>209</v>
       </c>
       <c r="Y26" s="2" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
     </row>
     <row r="27" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5065,7 +5086,7 @@
         <v>12</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E27" s="1" t="s">
         <v>19</v>
@@ -5074,61 +5095,61 @@
         <v>17</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="H27" s="1" t="s">
-        <v>454</v>
+        <v>438</v>
       </c>
       <c r="I27" s="1" t="s">
-        <v>483</v>
+        <v>467</v>
       </c>
       <c r="J27" s="1">
         <v>2</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="L27" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="M27" s="1" t="s">
-        <v>104</v>
+        <v>230</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>571</v>
       </c>
       <c r="N27" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="O27" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P27" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="Q27" s="1" t="s">
-        <v>107</v>
+        <v>234</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>573</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>574</v>
       </c>
       <c r="R27" s="1" t="s">
-        <v>455</v>
+        <v>439</v>
       </c>
       <c r="S27" s="1" t="s">
-        <v>129</v>
+        <v>113</v>
       </c>
       <c r="T27" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="U27" s="1" t="s">
-        <v>131</v>
+        <v>115</v>
       </c>
       <c r="V27" s="2" t="s">
-        <v>582</v>
+        <v>566</v>
       </c>
       <c r="W27" s="1" t="s">
-        <v>132</v>
+        <v>116</v>
       </c>
       <c r="X27" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
       <c r="Y27" s="1" t="s">
-        <v>133</v>
+        <v>117</v>
       </c>
     </row>
     <row r="28" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5142,7 +5163,7 @@
         <v>20</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E28" s="1" t="s">
         <v>19</v>
@@ -5154,55 +5175,55 @@
         <v>15</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>456</v>
+        <v>440</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>484</v>
+        <v>468</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="L28" s="1" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="M28" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="N28" s="1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O28" s="1" t="s">
-        <v>110</v>
+        <v>105</v>
+      </c>
+      <c r="O28" s="2" t="s">
+        <v>579</v>
       </c>
       <c r="P28" s="1" t="s">
-        <v>111</v>
+        <v>578</v>
       </c>
       <c r="Q28" s="1" t="s">
-        <v>112</v>
+        <v>580</v>
       </c>
       <c r="R28" s="1" t="s">
-        <v>457</v>
+        <v>441</v>
       </c>
       <c r="S28" s="1" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="T28" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="U28" s="1" t="s">
-        <v>135</v>
+        <v>119</v>
       </c>
       <c r="V28" s="2" t="s">
-        <v>583</v>
+        <v>567</v>
       </c>
       <c r="W28" s="1" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
       <c r="X28" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
       <c r="Y28" s="1" t="s">
-        <v>137</v>
+        <v>121</v>
       </c>
     </row>
     <row r="29" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5216,7 +5237,7 @@
         <v>12</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E29" s="1" t="s">
         <v>19</v>
@@ -5228,55 +5249,55 @@
         <v>16</v>
       </c>
       <c r="H29" s="1" t="s">
-        <v>458</v>
+        <v>442</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>485</v>
+        <v>469</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="L29" s="1" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="M29" s="1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="N29" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="O29" s="1" t="s">
+        <v>581</v>
+      </c>
+      <c r="P29" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="Q29" s="1" t="s">
+        <v>576</v>
+      </c>
+      <c r="R29" s="1" t="s">
+        <v>443</v>
+      </c>
+      <c r="S29" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="T29" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="O29" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="P29" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="Q29" s="1" t="s">
-        <v>117</v>
-      </c>
-      <c r="R29" s="1" t="s">
-        <v>459</v>
-      </c>
-      <c r="S29" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="T29" s="1" t="s">
-        <v>130</v>
-      </c>
       <c r="U29" s="1" t="s">
-        <v>139</v>
+        <v>123</v>
       </c>
       <c r="V29" s="2" t="s">
-        <v>584</v>
+        <v>568</v>
       </c>
       <c r="W29" s="1" t="s">
-        <v>140</v>
+        <v>124</v>
       </c>
       <c r="X29" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="Y29" s="1" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5290,7 +5311,7 @@
         <v>12</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E30" s="1" t="s">
         <v>19</v>
@@ -5302,52 +5323,52 @@
         <v>17</v>
       </c>
       <c r="I30" s="1" t="s">
-        <v>486</v>
+        <v>470</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="L30" s="1" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="M30" s="1" t="s">
-        <v>119</v>
+        <v>109</v>
       </c>
       <c r="N30" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="O30" s="1" t="s">
-        <v>121</v>
-      </c>
-      <c r="P30" s="1" t="s">
-        <v>122</v>
+        <v>110</v>
+      </c>
+      <c r="O30" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="P30" s="2" t="s">
+        <v>584</v>
       </c>
       <c r="Q30" s="1" t="s">
-        <v>123</v>
+        <v>575</v>
       </c>
       <c r="R30" s="1" t="s">
-        <v>460</v>
+        <v>444</v>
       </c>
       <c r="S30" s="1" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="T30" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="U30" s="1" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="V30" s="2" t="s">
-        <v>585</v>
+        <v>569</v>
       </c>
       <c r="W30" s="1" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="X30" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
       <c r="Y30" s="1" t="s">
-        <v>145</v>
+        <v>129</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5361,7 +5382,7 @@
         <v>12</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
       <c r="E31" s="1" t="s">
         <v>19</v>
@@ -5373,46 +5394,46 @@
         <v>18</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="L31" s="1" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="M31" s="1" t="s">
-        <v>124</v>
+        <v>111</v>
       </c>
       <c r="N31" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="O31" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="P31" s="1" t="s">
-        <v>127</v>
+        <v>112</v>
+      </c>
+      <c r="O31" s="2" t="s">
+        <v>585</v>
+      </c>
+      <c r="P31" s="2" t="s">
+        <v>586</v>
       </c>
       <c r="Q31" s="1" t="s">
-        <v>128</v>
+        <v>577</v>
       </c>
       <c r="S31" s="1" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="T31" s="1" t="s">
-        <v>130</v>
+        <v>114</v>
       </c>
       <c r="U31" s="1" t="s">
-        <v>147</v>
+        <v>131</v>
       </c>
       <c r="V31" s="2" t="s">
-        <v>586</v>
+        <v>570</v>
       </c>
       <c r="W31" s="1" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="X31" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
       <c r="Y31" s="1" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5426,7 +5447,7 @@
         <v>12</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E32" s="1" t="s">
         <v>14</v>
@@ -5435,58 +5456,58 @@
         <v>16</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="H32" s="1" t="s">
-        <v>461</v>
+        <v>445</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>487</v>
+        <v>471</v>
       </c>
       <c r="J32" s="1">
         <v>5</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="L32" s="1" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="M32" s="1" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="N32" s="1" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="P32" s="1" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="Q32" s="1" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="S32" s="1" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="T32" s="1" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="U32" s="1" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="V32" s="1" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="W32" s="1" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="X32" s="1" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="Y32" s="1" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
     </row>
     <row r="33" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5500,7 +5521,7 @@
         <v>12</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E33" s="1" t="s">
         <v>14</v>
@@ -5512,52 +5533,52 @@
         <v>15</v>
       </c>
       <c r="H33" s="1" t="s">
-        <v>462</v>
+        <v>446</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>488</v>
+        <v>472</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="L33" s="1" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="O33" s="1" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="P33" s="1" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="Q33" s="1" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="S33" s="1" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="T33" s="1" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="U33" s="1" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="V33" s="1" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="W33" s="1" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="X33" s="1" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="Y33" s="1" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
     </row>
     <row r="34" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5571,7 +5592,7 @@
         <v>12</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>14</v>
@@ -5583,46 +5604,46 @@
         <v>16</v>
       </c>
       <c r="K34" s="1" t="s">
-        <v>326</v>
+        <v>310</v>
       </c>
       <c r="L34" s="1" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="M34" s="1" t="s">
-        <v>327</v>
+        <v>311</v>
       </c>
       <c r="N34" s="1" t="s">
-        <v>328</v>
+        <v>312</v>
       </c>
       <c r="O34" s="1" t="s">
-        <v>329</v>
+        <v>313</v>
       </c>
       <c r="P34" s="1" t="s">
-        <v>339</v>
+        <v>323</v>
       </c>
       <c r="Q34" s="1" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
       <c r="S34" s="1" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="T34" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="U34" s="1" t="s">
+        <v>281</v>
+      </c>
+      <c r="V34" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="W34" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="X34" s="1" t="s">
         <v>284</v>
       </c>
-      <c r="U34" s="1" t="s">
-        <v>297</v>
-      </c>
-      <c r="V34" s="1" t="s">
-        <v>298</v>
-      </c>
-      <c r="W34" s="1" t="s">
-        <v>299</v>
-      </c>
-      <c r="X34" s="1" t="s">
-        <v>300</v>
-      </c>
       <c r="Y34" s="1" t="s">
-        <v>301</v>
+        <v>285</v>
       </c>
     </row>
     <row r="35" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5636,7 +5657,7 @@
         <v>12</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>14</v>
@@ -5648,49 +5669,49 @@
         <v>17</v>
       </c>
       <c r="I35" s="1" t="s">
-        <v>489</v>
+        <v>473</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>325</v>
+        <v>309</v>
       </c>
       <c r="L35" s="1" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="M35" s="1" t="s">
-        <v>324</v>
+        <v>308</v>
       </c>
       <c r="N35" s="1" t="s">
-        <v>323</v>
+        <v>307</v>
       </c>
       <c r="O35" s="1" t="s">
-        <v>322</v>
+        <v>306</v>
       </c>
       <c r="P35" s="1" t="s">
-        <v>321</v>
+        <v>305</v>
       </c>
       <c r="Q35" s="1" t="s">
-        <v>320</v>
+        <v>304</v>
       </c>
       <c r="S35" s="1" t="s">
-        <v>307</v>
+        <v>291</v>
       </c>
       <c r="T35" s="1" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="U35" s="1" t="s">
-        <v>306</v>
+        <v>290</v>
       </c>
       <c r="V35" s="1" t="s">
-        <v>305</v>
+        <v>289</v>
       </c>
       <c r="W35" s="1" t="s">
-        <v>304</v>
+        <v>288</v>
       </c>
       <c r="X35" s="1" t="s">
-        <v>303</v>
+        <v>287</v>
       </c>
       <c r="Y35" s="1" t="s">
-        <v>302</v>
+        <v>286</v>
       </c>
     </row>
     <row r="36" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5704,7 +5725,7 @@
         <v>12</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E36" s="1" t="s">
         <v>14</v>
@@ -5716,46 +5737,46 @@
         <v>18</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>314</v>
+        <v>298</v>
       </c>
       <c r="L36" s="1" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="M36" s="1" t="s">
-        <v>315</v>
+        <v>299</v>
       </c>
       <c r="N36" s="1" t="s">
-        <v>316</v>
+        <v>300</v>
       </c>
       <c r="O36" s="1" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="P36" s="1" t="s">
-        <v>318</v>
+        <v>302</v>
       </c>
       <c r="Q36" s="1" t="s">
-        <v>319</v>
+        <v>303</v>
       </c>
       <c r="S36" s="1" t="s">
-        <v>308</v>
+        <v>292</v>
       </c>
       <c r="T36" s="1" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="U36" s="1" t="s">
-        <v>309</v>
+        <v>293</v>
       </c>
       <c r="V36" s="1" t="s">
-        <v>310</v>
+        <v>294</v>
       </c>
       <c r="W36" s="1" t="s">
-        <v>311</v>
+        <v>295</v>
       </c>
       <c r="X36" s="1" t="s">
-        <v>312</v>
+        <v>296</v>
       </c>
       <c r="Y36" s="1" t="s">
-        <v>313</v>
+        <v>297</v>
       </c>
     </row>
     <row r="37" spans="1:25" ht="114" customHeight="1" x14ac:dyDescent="0.85">
@@ -5769,7 +5790,7 @@
         <v>12</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E37" s="1" t="s">
         <v>19</v>
@@ -5778,13 +5799,13 @@
         <v>17</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>405</v>
+        <v>389</v>
       </c>
       <c r="H37" s="1" t="s">
-        <v>466</v>
+        <v>450</v>
       </c>
       <c r="I37" s="1" t="s">
-        <v>490</v>
+        <v>474</v>
       </c>
       <c r="J37" s="1">
         <v>1</v>
@@ -5811,7 +5832,7 @@
         <v>79</v>
       </c>
       <c r="R37" s="1" t="s">
-        <v>463</v>
+        <v>447</v>
       </c>
       <c r="S37" s="1" t="s">
         <v>42</v>
@@ -5846,7 +5867,7 @@
         <v>12</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>19</v>
@@ -5858,10 +5879,10 @@
         <v>15</v>
       </c>
       <c r="H38" s="1" t="s">
-        <v>464</v>
+        <v>448</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>491</v>
+        <v>475</v>
       </c>
       <c r="K38" s="1" t="s">
         <v>80</v>
@@ -5885,7 +5906,7 @@
         <v>85</v>
       </c>
       <c r="R38" s="1" t="s">
-        <v>465</v>
+        <v>449</v>
       </c>
       <c r="S38" s="1" t="s">
         <v>49</v>
@@ -5920,7 +5941,7 @@
         <v>12</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>19</v>
@@ -5985,7 +6006,7 @@
         <v>12</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E40" s="1" t="s">
         <v>19</v>
@@ -5997,7 +6018,7 @@
         <v>17</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>492</v>
+        <v>476</v>
       </c>
       <c r="K40" s="1" t="s">
         <v>92</v>
@@ -6021,7 +6042,7 @@
         <v>97</v>
       </c>
       <c r="R40" s="1" t="s">
-        <v>467</v>
+        <v>451</v>
       </c>
       <c r="S40" s="1" t="s">
         <v>61</v>
@@ -6056,7 +6077,7 @@
         <v>12</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
       <c r="E41" s="1" t="s">
         <v>19</v>
@@ -6187,7 +6208,6 @@
       <c r="H50"/>
       <c r="I50"/>
       <c r="J50"/>
-      <c r="K50"/>
       <c r="L50" s="2"/>
       <c r="M50" s="2"/>
       <c r="N50"/>
@@ -6777,6 +6797,141 @@
       <c r="H99"/>
       <c r="I99"/>
     </row>
+    <row r="100" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H100"/>
+    </row>
+    <row r="101" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H101"/>
+    </row>
+    <row r="102" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H102"/>
+    </row>
+    <row r="103" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H103"/>
+    </row>
+    <row r="104" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H104"/>
+    </row>
+    <row r="105" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H105"/>
+    </row>
+    <row r="106" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H106"/>
+    </row>
+    <row r="107" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H107"/>
+    </row>
+    <row r="108" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H108"/>
+    </row>
+    <row r="109" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H109"/>
+    </row>
+    <row r="110" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H110"/>
+    </row>
+    <row r="111" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H111"/>
+    </row>
+    <row r="112" spans="4:9" x14ac:dyDescent="0.85">
+      <c r="H112"/>
+    </row>
+    <row r="113" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H113"/>
+    </row>
+    <row r="114" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H114"/>
+    </row>
+    <row r="115" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H115"/>
+    </row>
+    <row r="116" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H116"/>
+    </row>
+    <row r="117" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H117"/>
+    </row>
+    <row r="118" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H118"/>
+    </row>
+    <row r="119" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H119"/>
+    </row>
+    <row r="120" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H120"/>
+    </row>
+    <row r="121" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H121"/>
+    </row>
+    <row r="122" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H122"/>
+    </row>
+    <row r="123" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H123"/>
+    </row>
+    <row r="124" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H124"/>
+    </row>
+    <row r="125" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H125"/>
+    </row>
+    <row r="126" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H126"/>
+    </row>
+    <row r="127" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H127"/>
+    </row>
+    <row r="128" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H128"/>
+    </row>
+    <row r="129" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H129"/>
+    </row>
+    <row r="130" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H130"/>
+    </row>
+    <row r="131" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H131"/>
+    </row>
+    <row r="132" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H132"/>
+    </row>
+    <row r="133" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H133"/>
+    </row>
+    <row r="134" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H134"/>
+    </row>
+    <row r="135" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H135"/>
+    </row>
+    <row r="136" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H136"/>
+    </row>
+    <row r="137" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H137"/>
+    </row>
+    <row r="138" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H138"/>
+    </row>
+    <row r="139" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H139"/>
+    </row>
+    <row r="140" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H140"/>
+    </row>
+    <row r="141" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H141"/>
+    </row>
+    <row r="142" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H142"/>
+    </row>
+    <row r="143" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H143"/>
+    </row>
+    <row r="144" spans="8:8" x14ac:dyDescent="0.85">
+      <c r="H144"/>
+    </row>
   </sheetData>
   <phoneticPr fontId="18"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>